<commit_message>
Sauvegarde - avant tri
</commit_message>
<xml_diff>
--- a/test_sampling_SD/networks/Square/models_config_Poisson2D_fixed2.xlsx
+++ b/test_sampling_SD/networks/Square/models_config_Poisson2D_fixed2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
   <si>
     <t>Configuration</t>
   </si>
@@ -109,13 +109,22 @@
     <t>1</t>
   </si>
   <si>
+    <t>20000</t>
+  </si>
+  <si>
     <t>2000</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
-    <t>20000</t>
+    <t>[10, 20, 60, 60, 20, 10]</t>
+  </si>
+  <si>
+    <t>[0.001]</t>
+  </si>
+  <si>
+    <t>10000</t>
   </si>
 </sst>
 </file>
@@ -245,7 +254,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9763125" y="571500"/>
+          <a:off x="9906000" y="571500"/>
           <a:ext cx="1371603" cy="731521"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -283,8 +292,84 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9763125" y="1333500"/>
+          <a:off x="9906000" y="1333500"/>
           <a:ext cx="1371603" cy="731521"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>914402</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>685801</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="corr_fem_1_exact_bc.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12668250" y="1333500"/>
+          <a:ext cx="914402" cy="685801"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>914402</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>685801</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="corr_phifem_1_exact_bc.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14630400" y="1333500"/>
+          <a:ext cx="914402" cy="685801"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -308,21 +393,97 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="model_2_exact_bc.png"/>
+        <xdr:cNvPr id="6" name="Picture 5" descr="model_2_exact_bc.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9763125" y="2095500"/>
+          <a:off x="9906000" y="2095500"/>
           <a:ext cx="1371603" cy="731521"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>914402</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>685801</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6" descr="corr_fem_2_exact_bc.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12668250" y="2095500"/>
+          <a:ext cx="914402" cy="685801"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>914402</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>685801</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7" descr="corr_phifem_2_exact_bc.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14630400" y="2095500"/>
+          <a:ext cx="914402" cy="685801"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -626,7 +787,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
@@ -820,14 +981,14 @@
       <c r="H5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>28</v>
+      <c r="I5" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>21</v>
@@ -841,16 +1002,16 @@
     </row>
     <row r="6" spans="1:18" ht="60" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>33</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>24</v>
+      <c r="D6" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>25</v>
@@ -864,14 +1025,14 @@
       <c r="H6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>31</v>
+      <c r="J6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>21</v>

</xml_diff>